<commit_message>
Se corrigió provedor en el catalogo
</commit_message>
<xml_diff>
--- a/Organización/Capacitacion/Plan_capacitacion2015.xlsx
+++ b/Organización/Capacitacion/Plan_capacitacion2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo de cursos" sheetId="7" r:id="rId1"/>
@@ -850,6 +850,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -861,9 +864,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1590,8 +1590,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,26 +1611,26 @@
     <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -1914,7 +1914,7 @@
         <v>131</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>131</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>131</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2018,7 +2018,7 @@
         <v>131</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2044,7 +2044,7 @@
         <v>131</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2070,7 +2070,7 @@
         <v>131</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
         <v>131</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,7 +2122,7 @@
         <v>131</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2148,7 +2148,7 @@
         <v>131</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -2178,7 +2178,7 @@
         <v>131</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -2208,7 +2208,7 @@
         <v>131</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
@@ -2238,7 +2238,7 @@
         <v>131</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
@@ -2268,7 +2268,7 @@
         <v>131</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
@@ -2298,7 +2298,7 @@
         <v>131</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
@@ -2328,7 +2328,7 @@
         <v>131</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
@@ -2358,7 +2358,7 @@
         <v>131</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
@@ -2388,7 +2388,7 @@
         <v>131</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -2598,8 +2598,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AZ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,36 +2640,36 @@
     </row>
     <row r="6" spans="1:52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -3149,7 +3149,7 @@
       <c r="D22" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="39" t="s">
         <v>162</v>
       </c>
       <c r="F22" s="31" t="s">
@@ -3226,7 +3226,7 @@
       <c r="D24" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="39" t="s">
         <v>162</v>
       </c>
       <c r="F24" s="31" t="s">
@@ -3814,16 +3814,16 @@
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
@@ -3890,44 +3890,44 @@
       <c r="D16" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3964,20 +3964,20 @@
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -4087,46 +4087,46 @@
       <c r="E20" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Se agregó un objetivo organizacional
</commit_message>
<xml_diff>
--- a/Organización/Capacitacion/Plan_capacitacion2015.xlsx
+++ b/Organización/Capacitacion/Plan_capacitacion2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogo de cursos" sheetId="7" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="160">
   <si>
     <t>PLAN DE CAPACITACIONES</t>
   </si>
@@ -217,9 +217,6 @@
 Monitorea la gestión de las capacitaciones.</t>
   </si>
   <si>
-    <t>[Ingrese el correo eléctronico del contacto]</t>
-  </si>
-  <si>
     <t>Costo del curso</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>Este  apartado  es  para  las  capacitaciones  que ya  se  aprobaron.</t>
   </si>
   <si>
-    <t>[Ingrese la dirección del contacto]</t>
-  </si>
-  <si>
     <t>Catalogo de cursos</t>
   </si>
   <si>
@@ -257,15 +251,6 @@
   </si>
   <si>
     <t>[Indica el tiempo que durara el curso]</t>
-  </si>
-  <si>
-    <t>[Ingresa el nombre del proveedor]</t>
-  </si>
-  <si>
-    <t>[Ingrese el nombre completo de la persona en contacto]</t>
-  </si>
-  <si>
-    <t>[Del contacto]</t>
   </si>
   <si>
     <t>Realizar taller de OPD y OPF</t>
@@ -591,13 +576,19 @@
   </si>
   <si>
     <t>29/05/2015                       10/07/2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objetivo organizacional: </t>
+  </si>
+  <si>
+    <t>Mantener a todo el equipo capacitado según las necesidades previas que aparescan con cada proyecto a desarrollar.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,6 +677,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -713,7 +720,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -737,9 +744,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </left>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -756,7 +770,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -805,12 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -864,6 +872,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1590,7 +1605,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AT49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+    <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
@@ -1611,30 +1626,30 @@
     <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
+      <c r="A7" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1645,510 +1660,510 @@
         <v>5</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>43</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>52</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>129</v>
+        <v>53</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>124</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>132</v>
+        <v>54</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>134</v>
+        <v>55</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>129</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>136</v>
+        <v>56</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>160</v>
+      <c r="E16" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>132</v>
+        <v>58</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>144</v>
+        <v>59</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>136</v>
+        <v>60</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>146</v>
+        <v>61</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>142</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>160</v>
+        <v>62</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>151</v>
+        <v>73</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>151</v>
+        <v>74</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>151</v>
+        <v>75</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>151</v>
+        <v>76</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>151</v>
+      <c r="A26" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>151</v>
+        <v>77</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>151</v>
+      <c r="A28" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>151</v>
+        <v>80</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -2157,28 +2172,28 @@
     </row>
     <row r="30" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" s="30" t="s">
-        <v>151</v>
+        <v>81</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -2187,28 +2202,28 @@
     </row>
     <row r="31" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>151</v>
+        <v>82</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
@@ -2217,28 +2232,28 @@
     </row>
     <row r="32" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="30" t="s">
-        <v>151</v>
+        <v>83</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
@@ -2247,28 +2262,28 @@
     </row>
     <row r="33" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>160</v>
+      <c r="E33" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
@@ -2277,28 +2292,28 @@
     </row>
     <row r="34" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>151</v>
+        <v>85</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
@@ -2307,28 +2322,28 @@
     </row>
     <row r="35" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>154</v>
+        <v>88</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>149</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
@@ -2337,28 +2352,28 @@
     </row>
     <row r="36" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C36" s="30" t="s">
-        <v>155</v>
+        <v>86</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>150</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
@@ -2367,28 +2382,28 @@
     </row>
     <row r="37" spans="1:12" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>157</v>
+        <v>87</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>152</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="38" t="s">
-        <v>160</v>
+        <v>89</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>155</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -2583,7 +2598,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Lista de Proveedores'!$A$11:$A$20</xm:f>
+            <xm:f>'Lista de Proveedores'!$A$11:$A$19</xm:f>
           </x14:formula1>
           <xm:sqref>H11</xm:sqref>
         </x14:dataValidation>
@@ -2640,47 +2655,47 @@
     </row>
     <row r="6" spans="1:52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:52" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2716,1061 +2731,1061 @@
       <c r="AZ10"/>
     </row>
     <row r="11" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25" t="s">
+      <c r="K11" s="23"/>
+      <c r="L11" s="23" t="s">
         <v>22</v>
       </c>
       <c r="AZ11"/>
     </row>
     <row r="12" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="28">
+        <v>62</v>
+      </c>
+      <c r="E12" s="26">
         <v>41961</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J12" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ12"/>
     </row>
     <row r="13" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="28">
+        <v>62</v>
+      </c>
+      <c r="E13" s="26">
         <v>41976</v>
       </c>
       <c r="F13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="AZ13"/>
     </row>
     <row r="14" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="28">
+        <v>62</v>
+      </c>
+      <c r="E14" s="26">
         <v>41989</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J14" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ14"/>
     </row>
     <row r="15" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J15" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J15" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ15"/>
     </row>
     <row r="16" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <v>42017</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J16" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ16"/>
     </row>
     <row r="17" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="C17" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="28">
+        <v>62</v>
+      </c>
+      <c r="E17" s="26">
         <v>42024</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ17"/>
     </row>
     <row r="18" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="26">
+        <v>42031</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="28">
-        <v>42031</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J18" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="L18" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ18"/>
     </row>
     <row r="19" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="28">
+        <v>62</v>
+      </c>
+      <c r="E19" s="26">
         <v>42045</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ19"/>
     </row>
     <row r="20" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="28">
+        <v>62</v>
+      </c>
+      <c r="E20" s="26">
         <v>42073</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="J20" s="32" t="s">
+        <v>94</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="AZ20"/>
     </row>
     <row r="21" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L21" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="AZ21"/>
     </row>
     <row r="22" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K22" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="F22" s="31" t="s">
+      <c r="L22" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="J22" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L22" s="31" t="s">
-        <v>101</v>
       </c>
       <c r="AZ22"/>
     </row>
     <row r="23" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="31">
+        <v>42154</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="33">
-        <v>42154</v>
-      </c>
-      <c r="F23" s="31" t="s">
+      <c r="L23" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J23" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K24" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="F24" s="31" t="s">
+      <c r="L24" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="I24" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="J24" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L24" s="31" t="s">
-        <v>101</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="31">
+        <v>42156</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K25" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="31" t="s">
+      <c r="L25" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" s="25"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="31">
+        <v>42157</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="33">
-        <v>42156</v>
-      </c>
-      <c r="F25" s="31" t="s">
+      <c r="K26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I25" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J25" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L25" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="M25" s="27"/>
-      <c r="N25" s="2"/>
-    </row>
-    <row r="26" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="33">
-        <v>42157</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H26" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I26" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L26" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="M26" s="27"/>
+      <c r="M26" s="25"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="31">
+        <v>42158</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K27" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="31" t="s">
+      <c r="L27" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="M27" s="25"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="31">
+        <v>42159</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="33">
-        <v>42158</v>
-      </c>
-      <c r="F27" s="31" t="s">
+      <c r="K28" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L28" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I27" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J27" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L27" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="M27" s="27"/>
-      <c r="N27" s="2"/>
-    </row>
-    <row r="28" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="33">
-        <v>42159</v>
-      </c>
-      <c r="F28" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I28" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L28" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="M28" s="27"/>
+      <c r="M28" s="25"/>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="31">
+        <v>42160</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K29" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="33">
-        <v>42160</v>
-      </c>
-      <c r="F29" s="31" t="s">
+      <c r="L29" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J29" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L29" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="M29" s="27"/>
+      <c r="M29" s="25"/>
       <c r="N29" s="2"/>
     </row>
     <row r="30" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="31">
+        <v>42161</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K30" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="33">
-        <v>42161</v>
-      </c>
-      <c r="F30" s="31" t="s">
+      <c r="L30" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I30" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J30" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L30" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="31">
+        <v>42162</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K31" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="33">
-        <v>42162</v>
-      </c>
-      <c r="F31" s="31" t="s">
+      <c r="L31" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I31" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J31" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L31" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:52" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="31">
+        <v>42163</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K32" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="33">
-        <v>42163</v>
-      </c>
-      <c r="F32" s="31" t="s">
+      <c r="L32" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I32" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J32" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L32" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="E33" s="31">
+        <v>42164</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K33" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="33">
-        <v>42164</v>
-      </c>
-      <c r="F33" s="31" t="s">
+      <c r="L33" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I33" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J33" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L33" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="C34" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="31">
+        <v>42165</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="K34" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="33">
-        <v>42165</v>
-      </c>
-      <c r="F34" s="31" t="s">
+      <c r="L34" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="I34" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J34" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L34" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="31">
+        <v>42166</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H35" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="J35" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="33">
-        <v>42166</v>
-      </c>
-      <c r="F35" s="31" t="s">
+      <c r="K35" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L35" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="I35" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="J35" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L35" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="31">
+        <v>42167</v>
+      </c>
+      <c r="F36" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B36" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" s="31" t="s">
+      <c r="G36" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I36" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="J36" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="33">
-        <v>42167</v>
-      </c>
-      <c r="F36" s="31" t="s">
+      <c r="K36" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L36" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H36" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I36" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="J36" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L36" s="31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="31">
+        <v>42168</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I37" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="J37" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="33">
-        <v>42168</v>
-      </c>
-      <c r="F37" s="31" t="s">
+      <c r="K37" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L37" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H37" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="J37" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L37" s="31" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="24"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="25"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="25"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="25"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
+      <c r="A45" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3795,13 +3810,13 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="56.28515625" customWidth="1"/>
     <col min="4" max="4" width="60" customWidth="1"/>
@@ -3814,25 +3829,34 @@
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-    </row>
-    <row r="10" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+    </row>
+    <row r="9" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="44"/>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3841,7 +3865,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>36</v>
@@ -3853,7 +3877,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>38</v>
@@ -3863,20 +3887,19 @@
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>96</v>
+      <c r="B13" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>40</v>
@@ -3890,49 +3913,50 @@
       <c r="D16" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A7:C8"/>
     <mergeCell ref="A19:C26"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3942,10 +3966,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E8"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,20 +3988,20 @@
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
@@ -3996,48 +4020,38 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" s="7">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="7">
         <v>333150296</v>
       </c>
-      <c r="E12" s="37" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="E11" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="35"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -4079,59 +4093,52 @@
       <c r="D19" s="7"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A7:E8"/>
-    <mergeCell ref="A23:E28"/>
+    <mergeCell ref="A22:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>